<commit_message>
run model to import intermediate structure
</commit_message>
<xml_diff>
--- a/asistente_ladm_col/resources/excel/datos_estructura_excel.xlsx
+++ b/asistente_ladm_col/resources/excel/datos_estructura_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="predio" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="236">
   <si>
     <t xml:space="preserve">departamento</t>
   </si>
@@ -56,9 +56,15 @@
     <t xml:space="preserve">avaluo</t>
   </si>
   <si>
+    <t xml:space="preserve">condicion predio</t>
+  </si>
+  <si>
     <t xml:space="preserve">tipo predio</t>
   </si>
   <si>
+    <t xml:space="preserve">direccion</t>
+  </si>
+  <si>
     <t xml:space="preserve">132440001000000030131000000000</t>
   </si>
   <si>
@@ -68,102 +74,159 @@
     <t xml:space="preserve">NPH</t>
   </si>
   <si>
+    <t xml:space="preserve">Privado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07 25</t>
+  </si>
+  <si>
     <t xml:space="preserve">132440001000000035041000000000</t>
   </si>
   <si>
     <t xml:space="preserve">13244000100035041000</t>
   </si>
   <si>
+    <t xml:space="preserve">9A 42</t>
+  </si>
+  <si>
     <t xml:space="preserve">705080002000000050015000000000</t>
   </si>
   <si>
     <t xml:space="preserve">70508000200050015000</t>
   </si>
   <si>
+    <t xml:space="preserve">9A 26</t>
+  </si>
+  <si>
     <t xml:space="preserve">705080002000000050023000000000</t>
   </si>
   <si>
     <t xml:space="preserve">70508000200050023000</t>
   </si>
   <si>
+    <t xml:space="preserve">9A 46</t>
+  </si>
+  <si>
     <t xml:space="preserve">705080002000000050048500000014</t>
   </si>
   <si>
     <t xml:space="preserve">70508000200050085015</t>
   </si>
   <si>
+    <t xml:space="preserve">9A 36</t>
+  </si>
+  <si>
     <t xml:space="preserve">705080002000000050134000000000</t>
   </si>
   <si>
     <t xml:space="preserve">70508000200050134000</t>
   </si>
   <si>
+    <t xml:space="preserve">9A 30</t>
+  </si>
+  <si>
     <t xml:space="preserve">705080002000000050136000000000</t>
   </si>
   <si>
     <t xml:space="preserve">70508000200050136000</t>
   </si>
   <si>
+    <t xml:space="preserve">9A 20</t>
+  </si>
+  <si>
     <t xml:space="preserve">705080002000000050147000000000</t>
   </si>
   <si>
     <t xml:space="preserve">70508000200050147000</t>
   </si>
   <si>
+    <t xml:space="preserve">9A 04</t>
+  </si>
+  <si>
     <t xml:space="preserve">705080002000000050154000000000</t>
   </si>
   <si>
     <t xml:space="preserve">70508000200050154000</t>
   </si>
   <si>
+    <t xml:space="preserve">9A 08</t>
+  </si>
+  <si>
     <t xml:space="preserve">705080002000000050162000000000</t>
   </si>
   <si>
     <t xml:space="preserve">70508000200050162000</t>
   </si>
   <si>
+    <t xml:space="preserve">9A 14</t>
+  </si>
+  <si>
     <t xml:space="preserve">705080002000000050181000000000</t>
   </si>
   <si>
     <t xml:space="preserve">70508000200050181000</t>
   </si>
   <si>
+    <t xml:space="preserve">13A 88</t>
+  </si>
+  <si>
     <t xml:space="preserve">705080002000000050187000000000</t>
   </si>
   <si>
     <t xml:space="preserve">70508000200050187000</t>
   </si>
   <si>
+    <t xml:space="preserve">09 50</t>
+  </si>
+  <si>
     <t xml:space="preserve">705080600000000060011000000000</t>
   </si>
   <si>
     <t xml:space="preserve">70508060000060011000</t>
   </si>
   <si>
+    <t xml:space="preserve">6A 13</t>
+  </si>
+  <si>
     <t xml:space="preserve">705080600000000070007000000000</t>
   </si>
   <si>
     <t xml:space="preserve">70508060000070007000</t>
   </si>
   <si>
+    <t xml:space="preserve">06 71</t>
+  </si>
+  <si>
     <t xml:space="preserve">705080600000000090004000000000</t>
   </si>
   <si>
     <t xml:space="preserve">70508060000090004000</t>
   </si>
   <si>
+    <t xml:space="preserve">7A 23</t>
+  </si>
+  <si>
     <t xml:space="preserve">705080600000000090006000000000</t>
   </si>
   <si>
     <t xml:space="preserve">70508060000090006000</t>
   </si>
   <si>
+    <t xml:space="preserve">Publico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN</t>
+  </si>
+  <si>
     <t xml:space="preserve">705080600000000090051000000000</t>
   </si>
   <si>
     <t xml:space="preserve">70508060000090051000</t>
   </si>
   <si>
+    <t xml:space="preserve">10 15</t>
+  </si>
+  <si>
     <t xml:space="preserve">nombre1</t>
   </si>
   <si>
@@ -446,187 +509,196 @@
     <t xml:space="preserve">25956665</t>
   </si>
   <si>
+    <t xml:space="preserve">Escritura_Publica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disponible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E:\DOWNLOADS\Ebers7766.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dominio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">943634</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documento_Privado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posesion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">942344</t>
+  </si>
+  <si>
+    <t xml:space="preserve">943646</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nuda_Propiedad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13891204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sentencia_Judicial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3921606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E:\DOWNLOADS\escritura-griega-antigua-cincelado-en-piedra.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3771432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23025748</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22862681</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23022646</t>
+  </si>
+  <si>
+    <t xml:space="preserve">943565</t>
+  </si>
+  <si>
+    <t xml:space="preserve">942753</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18880035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">973641</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4190877</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ilicode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PropiedadHorizontal.Matriz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PropiedadHorizontal.UnidadPredial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condominio.Matriz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condominio.UnidadPredial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mejora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ParqueCementerio.Matriz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ParqueCementerio.UnidadPrivada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Via</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BienUsoPublico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deposito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parqueadero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bodega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cedula_Extranjeria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasaporte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarjeta_Identidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Libreta_Militar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registro_Civil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cedula_Militar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secuencial_SNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secuencial_IGAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Persona_No_Natural</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descripción</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Derecho_Propiedad_Colectiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mineria_Derecho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tenencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usufructo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aplica para Propietario</t>
+  </si>
+  <si>
     <t xml:space="preserve">Escritura</t>
   </si>
   <si>
-    <t xml:space="preserve">Disponible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E:\DOWNLOADS\Ebers7766.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dominio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">943634</t>
+    <t xml:space="preserve">Certificado</t>
   </si>
   <si>
     <t xml:space="preserve">Contrato</t>
   </si>
   <si>
-    <t xml:space="preserve">Posesion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">942344</t>
-  </si>
-  <si>
-    <t xml:space="preserve">943646</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nuda_Propiedad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13891204</t>
+    <t xml:space="preserve">Documento_Identidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formulario_Predial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promesa_Compraventa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reglamento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolucion</t>
   </si>
   <si>
     <t xml:space="preserve">Sentencia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3921606</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E:\DOWNLOADS\escritura-griega-antigua-cincelado-en-piedra.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3771432</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23025748</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22862681</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23022646</t>
-  </si>
-  <si>
-    <t xml:space="preserve">943565</t>
-  </si>
-  <si>
-    <t xml:space="preserve">942753</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18880035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">973641</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4190877</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ilicode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PropiedadHorizontal.Matriz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PropiedadHorizontal.UnidadPredial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condominio.Matriz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condominio.UnidadPredial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mejora</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ParqueCementerio.Matriz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ParqueCementerio.UnidadPrivada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Via</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BienUsoPublico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deposito</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parqueadero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bodega</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cedula_Extranjeria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pasaporte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tarjeta_Identidad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Libreta_Militar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registro_Civil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cedula_Militar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secuencial_SNR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secuencial_IGAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Persona_No_Natural</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Otro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Derecho_Propiedad_Colectiva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mineria_Derecho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tenencia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usufructo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aplica para Propietario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Certificado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Documento_Identidad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Informe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Formulario_Predial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Promesa_Compraventa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reglamento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resolucion</t>
   </si>
   <si>
     <t xml:space="preserve">Solicitud</t>
@@ -680,6 +752,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -746,12 +819,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -761,10 +834,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -802,6 +875,12 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -811,13 +890,19 @@
         <v>244</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -828,13 +913,19 @@
         <v>244</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="0" t="s">
-        <v>11</v>
+      <c r="J3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -845,13 +936,19 @@
         <v>508</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>11</v>
+      <c r="K4" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -862,13 +959,19 @@
         <v>508</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -879,13 +982,19 @@
         <v>508</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -896,13 +1005,19 @@
         <v>508</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -913,13 +1028,19 @@
         <v>508</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -930,13 +1051,19 @@
         <v>508</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,13 +1074,19 @@
         <v>508</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -964,13 +1097,19 @@
         <v>508</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -981,13 +1120,19 @@
         <v>508</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -998,13 +1143,19 @@
         <v>508</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1015,13 +1166,19 @@
         <v>508</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1032,13 +1189,19 @@
         <v>508</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1049,13 +1212,19 @@
         <v>508</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,13 +1235,19 @@
         <v>508</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,13 +1258,19 @@
         <v>508</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1121,112 +1302,112 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>138</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>192</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>143</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>193</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>194</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>196</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>197</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>198</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>149</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -1258,22 +1439,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -1307,37 +1488,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="L1" s="0" t="s">
         <v>4</v>
@@ -1345,562 +1526,562 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>23025694</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>23025809</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>23025700</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>23025709</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>3917843</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>3921534</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>64890812</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>943616</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>973641</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>18880035</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C12" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="G12" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>25956665</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>92551342</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>3296895</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="D15" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="0" t="s">
-        <v>67</v>
-      </c>
       <c r="G15" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>942344</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>23025748</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>4190877</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>942753</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>3921606</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H20" s="0" t="n">
         <v>22862681</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>943646</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>943634</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H23" s="0" t="n">
         <v>943565</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H24" s="0" t="n">
         <v>23022646</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H25" s="0" t="n">
         <v>13891204</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="C26" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="F26" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="D26" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>67</v>
-      </c>
       <c r="G26" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>3771432</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1935,167 +2116,167 @@
         <v>4</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2116,14 +2297,14 @@
   </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="15"/>
@@ -2131,422 +2312,422 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>11</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>2721</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>741</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>737</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>1236</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>18</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>406</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>81</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>54</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>137</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>33</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>395</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>62</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>159</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>138</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>1646</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2578,72 +2759,72 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>173</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2675,62 +2856,62 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>177</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>179</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>180</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>181</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>182</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>183</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2762,22 +2943,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>184</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -2809,22 +2990,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -2856,53 +3037,53 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>186</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>187</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>188</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>190</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>191</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>